<commit_message>
Some Docker related Code
</commit_message>
<xml_diff>
--- a/src/main/resources/endpoints/URLS.xlsx
+++ b/src/main/resources/endpoints/URLS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10615"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gitanshgumpu/GitHub/SpringProject/src/main/resources/endpoints/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB98981-397A-0B47-94A4-2D694F3DE256}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{473D3B07-F35D-AD49-B26E-11F241F6E904}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18880" xr2:uid="{FF1B53F3-B647-4D4B-B329-A12724D37B91}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18740" xr2:uid="{FF1B53F3-B647-4D4B-B329-A12724D37B91}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -546,7 +546,7 @@
   <dimension ref="A5:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>